<commit_message>
dokoceny nejaky checky jak pro word tak writer
</commit_message>
<xml_diff>
--- a/23_fb750F.xlsx
+++ b/23_fb750F.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Projekty/bakalářská-práce/BP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA49217-29ED-F943-A429-46F067F32038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF049F4-FA81-0846-969D-BC0ABC5A9BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="19860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,6 @@
     <sheet name="data" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">data!$D$2:$D$23</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">data!$D$2:$D$23</definedName>
     <definedName name="hodnota">data!$E$28</definedName>
     <definedName name="pole">data!$E$30</definedName>
   </definedNames>
@@ -300,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -347,32 +345,14 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1818,7 +1798,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1832,7 +1812,7 @@
     <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1848,7 +1828,7 @@
       <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>